<commit_message>
feat: evolução tela login com fundo e imagens, correção erro relacional
</commit_message>
<xml_diff>
--- a/data/relatorios.xlsx
+++ b/data/relatorios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://giroprodutos-my.sharepoint.com/personal/cig360_giroprodutos_onmicrosoft_com/Documents/COMPARTILHADA - CIG360/02_RELATORIOS/09_PYTHON/ACESSO_WEB/CORE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://giroprodutos-my.sharepoint.com/personal/cig360_giroprodutos_onmicrosoft_com/Documents/COMPARTILHADA - CIG360/02_RELATORIOS/09_PYTHON/ACESSO_WEB/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_FCA29CDDF02444AE039C8665AA7DE59E473466BC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72198D57-390D-45E3-B97B-F9D4091BFBB7}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_FCA29CDDF02444AE039C8665AA7DE59E473466BC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4537BD76-7AB1-4BBD-AEA5-571392159253}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>nome_relatorio</t>
   </si>
@@ -37,18 +37,9 @@
     <t>Painel Recuperação</t>
   </si>
   <si>
-    <t>Fluxo de Caixa</t>
-  </si>
-  <si>
     <t>Painel Vendas</t>
   </si>
   <si>
-    <t>https://app.powerbi.com/view?r=eyJrIjoiMDY0ZWNlMGItMGE1MC00NjYxLWFmMzctNmVmY2RjNDc4YzllIiwidCI6ImM1M2UwMWZmLTQ5MjItNDAzYy1iZWE1LTQzOTZjMmUxMmQ5NyJ9</t>
-  </si>
-  <si>
-    <t>https://app.powerbi.com/view?r=eyJrIjoiNTI2MjI3NjctZDAwNy00NDc4LWI4NWMtZTg0ZjJmNjk1ZDk1IiwidCI6ImM1M2UwMWZmLTQ5MjItNDAzYy1iZWE1LTQzOTZjMmUxMmQ5NyJ9</t>
-  </si>
-  <si>
     <t>PowerBI</t>
   </si>
   <si>
@@ -59,6 +50,24 @@
   </si>
   <si>
     <t>relatorio_id</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiMTU3YWQxYjktYTI5MC00OTFmLWFlYzItYmZlMGZiZTRjNmVjIiwidCI6ImM1M2UwMWZmLTQ5MjItNDAzYy1iZWE1LTQzOTZjMmUxMmQ5NyJ9</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiZTg4MTQwNDEtNWFkYS00ZjY3LWEyMzItMjNlODczZGEyMDE3IiwidCI6ImM1M2UwMWZmLTQ5MjItNDAzYy1iZWE1LTQzOTZjMmUxMmQ5NyJ9</t>
+  </si>
+  <si>
+    <t>https://www.google.com/?hl=pt_BR</t>
+  </si>
+  <si>
+    <t>https://www.google.com/imghp?hl=pt-BR&amp;ogbl</t>
+  </si>
+  <si>
+    <t>Painel CIG Rentabilidade</t>
+  </si>
+  <si>
+    <t>Painel CIG Saldo Bancário</t>
   </si>
 </sst>
 </file>
@@ -442,13 +451,13 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -456,7 +465,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -476,16 +485,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -493,16 +502,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -510,16 +519,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -530,21 +539,21 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{3B77BBA7-8836-43FC-98B2-1BB3C41E66D5}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{DC8F47D9-72AC-4684-A7C7-414AAB4DE498}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{D87ABA5B-74BA-4AEF-BE08-217DFFB72B2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>